<commit_message>
Adjust Note Appearance from 2D to 3D, and try other outline effects...(not done yet)
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/Accelerate/Chart.xlsx
+++ b/Assets/StreamingAssets/Songs/Accelerate/Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\Bccelerate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\Accelerate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D6008D-0EFF-47C1-9FC0-81FA52A6729E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40E2E9A-990C-4DDD-BD6A-4D548B748C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="34">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,6 +152,10 @@
   </si>
   <si>
     <t>#63b8ff</t>
+  </si>
+  <si>
+    <t>Jagnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -533,7 +537,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -20470,15 +20474,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J338"/>
+  <dimension ref="A1:K338"/>
   <sheetViews>
-    <sheetView topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="L295" sqref="L295"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -20509,8 +20513,11 @@
       <c r="J1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20541,8 +20548,11 @@
       <c r="J2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -20573,8 +20583,11 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -20605,8 +20618,11 @@
       <c r="J4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -20637,8 +20653,11 @@
       <c r="J5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -20669,8 +20688,11 @@
       <c r="J6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -20701,8 +20723,11 @@
       <c r="J7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -20733,8 +20758,11 @@
       <c r="J8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -20765,8 +20793,11 @@
       <c r="J9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -20797,8 +20828,11 @@
       <c r="J10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -20829,8 +20863,11 @@
       <c r="J11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -20861,8 +20898,11 @@
       <c r="J12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -20893,8 +20933,11 @@
       <c r="J13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -20925,8 +20968,11 @@
       <c r="J14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -20957,8 +21003,11 @@
       <c r="J15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -20989,8 +21038,11 @@
       <c r="J16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -21021,8 +21073,11 @@
       <c r="J17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -21053,8 +21108,11 @@
       <c r="J18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -21085,8 +21143,11 @@
       <c r="J19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -21117,8 +21178,11 @@
       <c r="J20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -21149,8 +21213,11 @@
       <c r="J21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -21181,8 +21248,11 @@
       <c r="J22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -21213,8 +21283,11 @@
       <c r="J23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -21245,8 +21318,11 @@
       <c r="J24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -21277,8 +21353,11 @@
       <c r="J25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -21309,8 +21388,11 @@
       <c r="J26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -21341,8 +21423,11 @@
       <c r="J27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -21373,8 +21458,11 @@
       <c r="J28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -21405,8 +21493,11 @@
       <c r="J29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -21437,8 +21528,11 @@
       <c r="J30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -21469,8 +21563,11 @@
       <c r="J31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -21501,8 +21598,11 @@
       <c r="J32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -21533,8 +21633,11 @@
       <c r="J33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -21565,8 +21668,11 @@
       <c r="J34" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -21597,8 +21703,11 @@
       <c r="J35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -21629,8 +21738,11 @@
       <c r="J36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -21661,8 +21773,11 @@
       <c r="J37" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -21693,8 +21808,11 @@
       <c r="J38" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>6</v>
       </c>
@@ -21725,8 +21843,11 @@
       <c r="J39" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>7</v>
       </c>
@@ -21757,8 +21878,11 @@
       <c r="J40" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>8</v>
       </c>
@@ -21789,8 +21913,11 @@
       <c r="J41" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -21821,8 +21948,11 @@
       <c r="J42" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -21853,8 +21983,11 @@
       <c r="J43" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -21885,8 +22018,11 @@
       <c r="J44" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -21917,8 +22053,11 @@
       <c r="J45" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -21949,8 +22088,11 @@
       <c r="J46" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -21981,8 +22123,11 @@
       <c r="J47" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -22013,8 +22158,11 @@
       <c r="J48" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -22045,8 +22193,11 @@
       <c r="J49" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -22077,8 +22228,11 @@
       <c r="J50" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -22109,8 +22263,11 @@
       <c r="J51" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -22141,8 +22298,11 @@
       <c r="J52" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -22173,8 +22333,11 @@
       <c r="J53" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -22205,8 +22368,11 @@
       <c r="J54" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -22237,8 +22403,11 @@
       <c r="J55" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -22269,8 +22438,11 @@
       <c r="J56" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -22301,8 +22473,11 @@
       <c r="J57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -22333,8 +22508,11 @@
       <c r="J58" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -22365,8 +22543,11 @@
       <c r="J59" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -22397,8 +22578,11 @@
       <c r="J60" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -22429,8 +22613,11 @@
       <c r="J61" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -22461,8 +22648,11 @@
       <c r="J62" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -22493,8 +22683,11 @@
       <c r="J63" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -22525,8 +22718,11 @@
       <c r="J64" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3</v>
       </c>
@@ -22557,8 +22753,11 @@
       <c r="J65" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>3</v>
       </c>
@@ -22589,8 +22788,11 @@
       <c r="J66" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>3</v>
       </c>
@@ -22621,8 +22823,11 @@
       <c r="J67" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -22653,8 +22858,11 @@
       <c r="J68" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
@@ -22685,8 +22893,11 @@
       <c r="J69" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -22717,8 +22928,11 @@
       <c r="J70" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -22749,8 +22963,11 @@
       <c r="J71" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -22781,8 +22998,11 @@
       <c r="J72" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -22813,8 +23033,11 @@
       <c r="J73" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -22845,8 +23068,11 @@
       <c r="J74" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>17</v>
       </c>
@@ -22877,8 +23103,11 @@
       <c r="J75" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>17</v>
       </c>
@@ -22909,8 +23138,11 @@
       <c r="J76" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>17</v>
       </c>
@@ -22941,8 +23173,11 @@
       <c r="J77" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -22973,8 +23208,11 @@
       <c r="J78" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>17</v>
       </c>
@@ -23005,8 +23243,11 @@
       <c r="J79" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>17</v>
       </c>
@@ -23037,8 +23278,11 @@
       <c r="J80" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -23069,8 +23313,11 @@
       <c r="J81" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>17</v>
       </c>
@@ -23101,8 +23348,11 @@
       <c r="J82" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>17</v>
       </c>
@@ -23133,8 +23383,11 @@
       <c r="J83" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -23165,8 +23418,11 @@
       <c r="J84" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>17</v>
       </c>
@@ -23197,8 +23453,11 @@
       <c r="J85" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>17</v>
       </c>
@@ -23229,8 +23488,11 @@
       <c r="J86" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -23261,8 +23523,11 @@
       <c r="J87" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>17</v>
       </c>
@@ -23293,8 +23558,11 @@
       <c r="J88" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -23325,8 +23593,11 @@
       <c r="J89" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -23357,8 +23628,11 @@
       <c r="J90" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>17</v>
       </c>
@@ -23389,8 +23663,11 @@
       <c r="J91" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>17</v>
       </c>
@@ -23421,8 +23698,11 @@
       <c r="J92" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>17</v>
       </c>
@@ -23453,8 +23733,11 @@
       <c r="J93" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -23485,8 +23768,11 @@
       <c r="J94" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>17</v>
       </c>
@@ -23517,8 +23803,11 @@
       <c r="J95" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>17</v>
       </c>
@@ -23549,8 +23838,11 @@
       <c r="J96" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -23581,8 +23873,11 @@
       <c r="J97" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>17</v>
       </c>
@@ -23613,8 +23908,11 @@
       <c r="J98" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>17</v>
       </c>
@@ -23645,8 +23943,11 @@
       <c r="J99" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
@@ -23677,8 +23978,11 @@
       <c r="J100" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>17</v>
       </c>
@@ -23709,8 +24013,11 @@
       <c r="J101" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>17</v>
       </c>
@@ -23741,8 +24048,11 @@
       <c r="J102" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>17</v>
       </c>
@@ -23773,8 +24083,11 @@
       <c r="J103" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>17</v>
       </c>
@@ -23805,8 +24118,11 @@
       <c r="J104" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>17</v>
       </c>
@@ -23837,8 +24153,11 @@
       <c r="J105" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -23869,8 +24188,11 @@
       <c r="J106" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1</v>
       </c>
@@ -23901,8 +24223,11 @@
       <c r="J107" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1</v>
       </c>
@@ -23933,8 +24258,11 @@
       <c r="J108" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>17</v>
       </c>
@@ -23965,8 +24293,11 @@
       <c r="J109" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1</v>
       </c>
@@ -23997,8 +24328,11 @@
       <c r="J110" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>17</v>
       </c>
@@ -24029,8 +24363,11 @@
       <c r="J111" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>17</v>
       </c>
@@ -24061,8 +24398,11 @@
       <c r="J112" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -24093,8 +24433,11 @@
       <c r="J113" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>17</v>
       </c>
@@ -24125,8 +24468,11 @@
       <c r="J114" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>17</v>
       </c>
@@ -24157,8 +24503,11 @@
       <c r="J115" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>17</v>
       </c>
@@ -24189,8 +24538,11 @@
       <c r="J116" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>17</v>
       </c>
@@ -24221,8 +24573,11 @@
       <c r="J117" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>17</v>
       </c>
@@ -24253,8 +24608,11 @@
       <c r="J118" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1</v>
       </c>
@@ -24285,8 +24643,11 @@
       <c r="J119" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1</v>
       </c>
@@ -24317,8 +24678,11 @@
       <c r="J120" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1</v>
       </c>
@@ -24349,8 +24713,11 @@
       <c r="J121" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>17</v>
       </c>
@@ -24381,8 +24748,11 @@
       <c r="J122" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1</v>
       </c>
@@ -24413,8 +24783,11 @@
       <c r="J123" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>17</v>
       </c>
@@ -24445,8 +24818,11 @@
       <c r="J124" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>17</v>
       </c>
@@ -24477,8 +24853,11 @@
       <c r="J125" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1</v>
       </c>
@@ -24509,8 +24888,11 @@
       <c r="J126" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1</v>
       </c>
@@ -24541,8 +24923,11 @@
       <c r="J127" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>17</v>
       </c>
@@ -24573,8 +24958,11 @@
       <c r="J128" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>17</v>
       </c>
@@ -24605,8 +24993,11 @@
       <c r="J129" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>17</v>
       </c>
@@ -24637,8 +25028,11 @@
       <c r="J130" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>17</v>
       </c>
@@ -24669,8 +25063,11 @@
       <c r="J131" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>17</v>
       </c>
@@ -24701,8 +25098,11 @@
       <c r="J132" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1</v>
       </c>
@@ -24733,8 +25133,11 @@
       <c r="J133" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>17</v>
       </c>
@@ -24765,8 +25168,11 @@
       <c r="J134" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>17</v>
       </c>
@@ -24797,8 +25203,11 @@
       <c r="J135" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1</v>
       </c>
@@ -24829,8 +25238,11 @@
       <c r="J136" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>17</v>
       </c>
@@ -24861,8 +25273,11 @@
       <c r="J137" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>17</v>
       </c>
@@ -24893,8 +25308,11 @@
       <c r="J138" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>17</v>
       </c>
@@ -24925,8 +25343,11 @@
       <c r="J139" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>17</v>
       </c>
@@ -24957,8 +25378,11 @@
       <c r="J140" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>17</v>
       </c>
@@ -24989,8 +25413,11 @@
       <c r="J141" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1</v>
       </c>
@@ -25021,8 +25448,11 @@
       <c r="J142" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1</v>
       </c>
@@ -25053,8 +25483,11 @@
       <c r="J143" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1</v>
       </c>
@@ -25085,8 +25518,11 @@
       <c r="J144" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>17</v>
       </c>
@@ -25117,8 +25553,11 @@
       <c r="J145" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1</v>
       </c>
@@ -25149,8 +25588,11 @@
       <c r="J146" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1</v>
       </c>
@@ -25181,8 +25623,11 @@
       <c r="J147" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1</v>
       </c>
@@ -25213,8 +25658,11 @@
       <c r="J148" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>17</v>
       </c>
@@ -25245,8 +25693,11 @@
       <c r="J149" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>17</v>
       </c>
@@ -25277,8 +25728,11 @@
       <c r="J150" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1</v>
       </c>
@@ -25309,8 +25763,11 @@
       <c r="J151" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>1</v>
       </c>
@@ -25341,8 +25798,11 @@
       <c r="J152" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1</v>
       </c>
@@ -25373,8 +25833,11 @@
       <c r="J153" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>17</v>
       </c>
@@ -25405,8 +25868,11 @@
       <c r="J154" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>17</v>
       </c>
@@ -25437,8 +25903,11 @@
       <c r="J155" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>17</v>
       </c>
@@ -25469,8 +25938,11 @@
       <c r="J156" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>1</v>
       </c>
@@ -25501,8 +25973,11 @@
       <c r="J157" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>17</v>
       </c>
@@ -25533,8 +26008,11 @@
       <c r="J158" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1</v>
       </c>
@@ -25565,8 +26043,11 @@
       <c r="J159" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>17</v>
       </c>
@@ -25597,8 +26078,11 @@
       <c r="J160" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>17</v>
       </c>
@@ -25629,8 +26113,11 @@
       <c r="J161" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>17</v>
       </c>
@@ -25661,8 +26148,11 @@
       <c r="J162" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>17</v>
       </c>
@@ -25693,8 +26183,11 @@
       <c r="J163" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1</v>
       </c>
@@ -25725,8 +26218,11 @@
       <c r="J164" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1</v>
       </c>
@@ -25757,8 +26253,11 @@
       <c r="J165" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>17</v>
       </c>
@@ -25789,8 +26288,11 @@
       <c r="J166" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>17</v>
       </c>
@@ -25821,8 +26323,11 @@
       <c r="J167" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>17</v>
       </c>
@@ -25853,8 +26358,11 @@
       <c r="J168" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>17</v>
       </c>
@@ -25885,8 +26393,11 @@
       <c r="J169" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>1</v>
       </c>
@@ -25917,8 +26428,11 @@
       <c r="J170" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1</v>
       </c>
@@ -25949,8 +26463,11 @@
       <c r="J171" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1</v>
       </c>
@@ -25981,8 +26498,11 @@
       <c r="J172" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1</v>
       </c>
@@ -26013,8 +26533,11 @@
       <c r="J173" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1</v>
       </c>
@@ -26045,8 +26568,11 @@
       <c r="J174" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>17</v>
       </c>
@@ -26077,8 +26603,11 @@
       <c r="J175" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>17</v>
       </c>
@@ -26109,8 +26638,11 @@
       <c r="J176" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>17</v>
       </c>
@@ -26141,8 +26673,11 @@
       <c r="J177" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>17</v>
       </c>
@@ -26173,8 +26708,11 @@
       <c r="J178" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>1</v>
       </c>
@@ -26205,8 +26743,11 @@
       <c r="J179" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>1</v>
       </c>
@@ -26237,8 +26778,11 @@
       <c r="J180" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>1</v>
       </c>
@@ -26269,8 +26813,11 @@
       <c r="J181" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>1</v>
       </c>
@@ -26301,8 +26848,11 @@
       <c r="J182" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>1</v>
       </c>
@@ -26333,8 +26883,11 @@
       <c r="J183" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>1</v>
       </c>
@@ -26365,8 +26918,11 @@
       <c r="J184" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>17</v>
       </c>
@@ -26397,8 +26953,11 @@
       <c r="J185" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>1</v>
       </c>
@@ -26429,8 +26988,11 @@
       <c r="J186" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>17</v>
       </c>
@@ -26461,8 +27023,11 @@
       <c r="J187" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>1</v>
       </c>
@@ -26493,8 +27058,11 @@
       <c r="J188" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>1</v>
       </c>
@@ -26525,8 +27093,11 @@
       <c r="J189" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>17</v>
       </c>
@@ -26557,8 +27128,11 @@
       <c r="J190" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>1</v>
       </c>
@@ -26589,8 +27163,11 @@
       <c r="J191" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>1</v>
       </c>
@@ -26621,8 +27198,11 @@
       <c r="J192" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>17</v>
       </c>
@@ -26653,8 +27233,11 @@
       <c r="J193" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>17</v>
       </c>
@@ -26685,8 +27268,11 @@
       <c r="J194" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>17</v>
       </c>
@@ -26717,8 +27303,11 @@
       <c r="J195" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>17</v>
       </c>
@@ -26749,8 +27338,11 @@
       <c r="J196" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>17</v>
       </c>
@@ -26781,8 +27373,11 @@
       <c r="J197" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>1</v>
       </c>
@@ -26813,8 +27408,11 @@
       <c r="J198" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>17</v>
       </c>
@@ -26845,8 +27443,11 @@
       <c r="J199" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>17</v>
       </c>
@@ -26877,8 +27478,11 @@
       <c r="J200" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>1</v>
       </c>
@@ -26909,8 +27513,11 @@
       <c r="J201" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1</v>
       </c>
@@ -26941,8 +27548,11 @@
       <c r="J202" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1</v>
       </c>
@@ -26973,8 +27583,11 @@
       <c r="J203" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1</v>
       </c>
@@ -27005,8 +27618,11 @@
       <c r="J204" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1</v>
       </c>
@@ -27037,8 +27653,11 @@
       <c r="J205" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1</v>
       </c>
@@ -27069,8 +27688,11 @@
       <c r="J206" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1</v>
       </c>
@@ -27101,8 +27723,11 @@
       <c r="J207" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>1</v>
       </c>
@@ -27133,8 +27758,11 @@
       <c r="J208" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1</v>
       </c>
@@ -27165,8 +27793,11 @@
       <c r="J209" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>17</v>
       </c>
@@ -27197,8 +27828,11 @@
       <c r="J210" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>17</v>
       </c>
@@ -27229,8 +27863,11 @@
       <c r="J211" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>17</v>
       </c>
@@ -27261,8 +27898,11 @@
       <c r="J212" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>17</v>
       </c>
@@ -27293,8 +27933,11 @@
       <c r="J213" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>17</v>
       </c>
@@ -27325,8 +27968,11 @@
       <c r="J214" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>17</v>
       </c>
@@ -27357,8 +28003,11 @@
       <c r="J215" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>17</v>
       </c>
@@ -27389,8 +28038,11 @@
       <c r="J216" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>17</v>
       </c>
@@ -27421,8 +28073,11 @@
       <c r="J217" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>17</v>
       </c>
@@ -27453,8 +28108,11 @@
       <c r="J218" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>17</v>
       </c>
@@ -27485,8 +28143,11 @@
       <c r="J219" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>1</v>
       </c>
@@ -27517,8 +28178,11 @@
       <c r="J220" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>1</v>
       </c>
@@ -27549,8 +28213,11 @@
       <c r="J221" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>1</v>
       </c>
@@ -27581,8 +28248,11 @@
       <c r="J222" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>1</v>
       </c>
@@ -27613,8 +28283,11 @@
       <c r="J223" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>1</v>
       </c>
@@ -27645,8 +28318,11 @@
       <c r="J224" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>17</v>
       </c>
@@ -27677,8 +28353,11 @@
       <c r="J225" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>17</v>
       </c>
@@ -27709,8 +28388,11 @@
       <c r="J226" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>17</v>
       </c>
@@ -27741,8 +28423,11 @@
       <c r="J227" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>1</v>
       </c>
@@ -27773,8 +28458,11 @@
       <c r="J228" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>1</v>
       </c>
@@ -27805,8 +28493,11 @@
       <c r="J229" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>17</v>
       </c>
@@ -27837,8 +28528,11 @@
       <c r="J230" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>17</v>
       </c>
@@ -27869,8 +28563,11 @@
       <c r="J231" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>17</v>
       </c>
@@ -27901,8 +28598,11 @@
       <c r="J232" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>17</v>
       </c>
@@ -27933,8 +28633,11 @@
       <c r="J233" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>17</v>
       </c>
@@ -27965,8 +28668,11 @@
       <c r="J234" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>17</v>
       </c>
@@ -27997,8 +28703,11 @@
       <c r="J235" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>17</v>
       </c>
@@ -28029,8 +28738,11 @@
       <c r="J236" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>17</v>
       </c>
@@ -28061,8 +28773,11 @@
       <c r="J237" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>17</v>
       </c>
@@ -28093,8 +28808,11 @@
       <c r="J238" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>17</v>
       </c>
@@ -28125,8 +28843,11 @@
       <c r="J239" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>1</v>
       </c>
@@ -28157,8 +28878,11 @@
       <c r="J240" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>1</v>
       </c>
@@ -28189,8 +28913,11 @@
       <c r="J241" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>1</v>
       </c>
@@ -28221,8 +28948,11 @@
       <c r="J242" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>1</v>
       </c>
@@ -28253,8 +28983,11 @@
       <c r="J243" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>17</v>
       </c>
@@ -28285,8 +29018,11 @@
       <c r="J244" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>17</v>
       </c>
@@ -28317,8 +29053,11 @@
       <c r="J245" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>17</v>
       </c>
@@ -28349,8 +29088,11 @@
       <c r="J246" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>17</v>
       </c>
@@ -28381,8 +29123,11 @@
       <c r="J247" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>17</v>
       </c>
@@ -28413,8 +29158,11 @@
       <c r="J248" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>17</v>
       </c>
@@ -28445,8 +29193,11 @@
       <c r="J249" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>19</v>
       </c>
@@ -28477,8 +29228,11 @@
       <c r="J250" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>19</v>
       </c>
@@ -28509,8 +29263,11 @@
       <c r="J251" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>19</v>
       </c>
@@ -28541,8 +29298,11 @@
       <c r="J252" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>19</v>
       </c>
@@ -28573,8 +29333,11 @@
       <c r="J253" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>19</v>
       </c>
@@ -28605,8 +29368,11 @@
       <c r="J254" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>17</v>
       </c>
@@ -28637,8 +29403,11 @@
       <c r="J255" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>19</v>
       </c>
@@ -28669,8 +29438,11 @@
       <c r="J256" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>19</v>
       </c>
@@ -28701,8 +29473,11 @@
       <c r="J257" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>19</v>
       </c>
@@ -28733,8 +29508,11 @@
       <c r="J258" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>19</v>
       </c>
@@ -28765,8 +29543,11 @@
       <c r="J259" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>17</v>
       </c>
@@ -28797,8 +29578,11 @@
       <c r="J260" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>19</v>
       </c>
@@ -28829,8 +29613,11 @@
       <c r="J261" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>17</v>
       </c>
@@ -28861,8 +29648,11 @@
       <c r="J262" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>19</v>
       </c>
@@ -28893,8 +29683,11 @@
       <c r="J263" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>17</v>
       </c>
@@ -28925,8 +29718,11 @@
       <c r="J264" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>19</v>
       </c>
@@ -28957,8 +29753,11 @@
       <c r="J265" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>17</v>
       </c>
@@ -28989,8 +29788,11 @@
       <c r="J266" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>17</v>
       </c>
@@ -29021,8 +29823,11 @@
       <c r="J267" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>19</v>
       </c>
@@ -29053,8 +29858,11 @@
       <c r="J268" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>19</v>
       </c>
@@ -29085,8 +29893,11 @@
       <c r="J269" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>17</v>
       </c>
@@ -29117,8 +29928,11 @@
       <c r="J270" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>17</v>
       </c>
@@ -29149,8 +29963,11 @@
       <c r="J271" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>19</v>
       </c>
@@ -29181,8 +29998,11 @@
       <c r="J272" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>19</v>
       </c>
@@ -29213,8 +30033,11 @@
       <c r="J273" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>19</v>
       </c>
@@ -29245,8 +30068,11 @@
       <c r="J274" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>19</v>
       </c>
@@ -29277,8 +30103,11 @@
       <c r="J275" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>19</v>
       </c>
@@ -29309,8 +30138,11 @@
       <c r="J276" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>17</v>
       </c>
@@ -29341,8 +30173,11 @@
       <c r="J277" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>19</v>
       </c>
@@ -29373,8 +30208,11 @@
       <c r="J278" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>19</v>
       </c>
@@ -29405,8 +30243,11 @@
       <c r="J279" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>19</v>
       </c>
@@ -29437,8 +30278,11 @@
       <c r="J280" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>19</v>
       </c>
@@ -29469,8 +30313,11 @@
       <c r="J281" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>17</v>
       </c>
@@ -29501,8 +30348,11 @@
       <c r="J282" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>19</v>
       </c>
@@ -29533,8 +30383,11 @@
       <c r="J283" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>17</v>
       </c>
@@ -29565,8 +30418,11 @@
       <c r="J284" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>19</v>
       </c>
@@ -29597,8 +30453,11 @@
       <c r="J285" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>17</v>
       </c>
@@ -29629,8 +30488,11 @@
       <c r="J286" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>19</v>
       </c>
@@ -29661,8 +30523,11 @@
       <c r="J287" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>19</v>
       </c>
@@ -29693,8 +30558,11 @@
       <c r="J288" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>19</v>
       </c>
@@ -29725,8 +30593,11 @@
       <c r="J289" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>19</v>
       </c>
@@ -29757,8 +30628,11 @@
       <c r="J290" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>19</v>
       </c>
@@ -29789,8 +30663,11 @@
       <c r="J291" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>17</v>
       </c>
@@ -29821,8 +30698,11 @@
       <c r="J292" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>19</v>
       </c>
@@ -29853,8 +30733,11 @@
       <c r="J293" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>17</v>
       </c>
@@ -29885,8 +30768,11 @@
       <c r="J294" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>19</v>
       </c>
@@ -29917,8 +30803,11 @@
       <c r="J295" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>19</v>
       </c>
@@ -29949,8 +30838,11 @@
       <c r="J296" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>19</v>
       </c>
@@ -29981,8 +30873,11 @@
       <c r="J297" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>19</v>
       </c>
@@ -30013,8 +30908,11 @@
       <c r="J298" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>19</v>
       </c>
@@ -30045,8 +30943,11 @@
       <c r="J299" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>19</v>
       </c>
@@ -30077,8 +30978,11 @@
       <c r="J300" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>19</v>
       </c>
@@ -30109,8 +31013,11 @@
       <c r="J301" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>19</v>
       </c>
@@ -30141,8 +31048,11 @@
       <c r="J302" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>19</v>
       </c>
@@ -30173,8 +31083,11 @@
       <c r="J303" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>19</v>
       </c>
@@ -30205,8 +31118,11 @@
       <c r="J304" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>19</v>
       </c>
@@ -30237,8 +31153,11 @@
       <c r="J305" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>19</v>
       </c>
@@ -30269,8 +31188,11 @@
       <c r="J306" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>19</v>
       </c>
@@ -30301,8 +31223,11 @@
       <c r="J307" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>19</v>
       </c>
@@ -30333,8 +31258,11 @@
       <c r="J308" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>17</v>
       </c>
@@ -30365,8 +31293,11 @@
       <c r="J309" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>19</v>
       </c>
@@ -30397,8 +31328,11 @@
       <c r="J310" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>17</v>
       </c>
@@ -30429,8 +31363,11 @@
       <c r="J311" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>19</v>
       </c>
@@ -30461,8 +31398,11 @@
       <c r="J312" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>19</v>
       </c>
@@ -30493,8 +31433,11 @@
       <c r="J313" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>19</v>
       </c>
@@ -30525,8 +31468,11 @@
       <c r="J314" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>19</v>
       </c>
@@ -30557,8 +31503,11 @@
       <c r="J315" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>19</v>
       </c>
@@ -30589,8 +31538,11 @@
       <c r="J316" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>19</v>
       </c>
@@ -30621,8 +31573,11 @@
       <c r="J317" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>19</v>
       </c>
@@ -30653,8 +31608,11 @@
       <c r="J318" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>19</v>
       </c>
@@ -30685,8 +31643,11 @@
       <c r="J319" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>19</v>
       </c>
@@ -30717,8 +31678,11 @@
       <c r="J320" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>17</v>
       </c>
@@ -30749,8 +31713,11 @@
       <c r="J321" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>17</v>
       </c>
@@ -30781,8 +31748,11 @@
       <c r="J322" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>17</v>
       </c>
@@ -30813,8 +31783,11 @@
       <c r="J323" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>17</v>
       </c>
@@ -30845,8 +31818,11 @@
       <c r="J324" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>17</v>
       </c>
@@ -30877,8 +31853,11 @@
       <c r="J325" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>17</v>
       </c>
@@ -30909,8 +31888,11 @@
       <c r="J326" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>19</v>
       </c>
@@ -30941,8 +31923,11 @@
       <c r="J327" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>19</v>
       </c>
@@ -30973,8 +31958,11 @@
       <c r="J328" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>17</v>
       </c>
@@ -31005,8 +31993,11 @@
       <c r="J329" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>17</v>
       </c>
@@ -31037,8 +32028,11 @@
       <c r="J330" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>17</v>
       </c>
@@ -31069,8 +32063,11 @@
       <c r="J331" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>17</v>
       </c>
@@ -31101,8 +32098,11 @@
       <c r="J332" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>17</v>
       </c>
@@ -31133,8 +32133,11 @@
       <c r="J333" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>17</v>
       </c>
@@ -31165,8 +32168,11 @@
       <c r="J334" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>19</v>
       </c>
@@ -31197,8 +32203,11 @@
       <c r="J335" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>19</v>
       </c>
@@ -31229,8 +32238,11 @@
       <c r="J336" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>19</v>
       </c>
@@ -31261,8 +32273,11 @@
       <c r="J337" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>19</v>
       </c>
@@ -31292,6 +32307,9 @@
       </c>
       <c r="J338" t="s">
         <v>26</v>
+      </c>
+      <c r="K338">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A complete version of outline effect (Render order not fixed..)
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/Accelerate/Chart.xlsx
+++ b/Assets/StreamingAssets/Songs/Accelerate/Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\Accelerate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40E2E9A-990C-4DDD-BD6A-4D548B748C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F91C4D-C528-489D-BA14-2448573572AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="35">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,9 +145,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#8ee5ee</t>
-  </si>
-  <si>
     <t>#dda0dd</t>
   </si>
   <si>
@@ -155,6 +152,13 @@
   </si>
   <si>
     <t>Jagnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#f0ffff</t>
+  </si>
+  <si>
+    <t>#f0ffff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -210,7 +214,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -219,6 +223,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,8 +544,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -565,13 +572,20 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,$I$1:$J$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -588,14 +602,21 @@
       <c r="G2" t="s">
         <v>23</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">VLOOKUP(A3,$I$1:$J$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C3">
         <v>0.42699999999999999</v>
@@ -612,14 +633,21 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C4">
         <v>1.246</v>
@@ -636,14 +664,21 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C5">
         <v>3.246</v>
@@ -659,6 +694,12 @@
       </c>
       <c r="G5" t="s">
         <v>23</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -666,8 +707,9 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C6">
         <v>1.246</v>
@@ -684,14 +726,21 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>32</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C7">
         <v>6.4450000000000003</v>
@@ -707,6 +756,12 @@
       </c>
       <c r="G7" t="s">
         <v>24</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -714,8 +769,9 @@
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C8">
         <v>6.4450000000000003</v>
@@ -732,14 +788,21 @@
       <c r="G8" t="s">
         <v>24</v>
       </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C9">
         <v>8.0259999999999998</v>
@@ -755,6 +818,12 @@
       </c>
       <c r="G9" t="s">
         <v>23</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -762,8 +831,9 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C10">
         <v>8.0259999999999998</v>
@@ -780,14 +850,21 @@
       <c r="G10" t="s">
         <v>23</v>
       </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
-        <v>32</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C11">
         <v>10.036</v>
@@ -803,6 +880,12 @@
       </c>
       <c r="G11" t="s">
         <v>23</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -810,8 +893,9 @@
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C12">
         <v>10.036</v>
@@ -828,14 +912,21 @@
       <c r="G12" t="s">
         <v>23</v>
       </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C13">
         <v>10.135999999999999</v>
@@ -851,6 +942,12 @@
       </c>
       <c r="G13" t="s">
         <v>23</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -858,8 +955,9 @@
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C14">
         <v>10.135999999999999</v>
@@ -876,14 +974,21 @@
       <c r="G14" t="s">
         <v>23</v>
       </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C15">
         <v>13.236000000000001</v>
@@ -899,6 +1004,12 @@
       </c>
       <c r="G15" t="s">
         <v>23</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -906,8 +1017,9 @@
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>30</v>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C16">
         <v>13.236000000000001</v>
@@ -924,14 +1036,21 @@
       <c r="G16" t="s">
         <v>23</v>
       </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>32</v>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C17">
         <v>13.336</v>
@@ -947,6 +1066,12 @@
       </c>
       <c r="G17" t="s">
         <v>23</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L17" s="2"/>
     </row>
@@ -954,8 +1079,9 @@
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C18">
         <v>13.336</v>
@@ -972,14 +1098,21 @@
       <c r="G18" t="s">
         <v>23</v>
       </c>
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>32</v>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C19">
         <v>16.436</v>
@@ -995,6 +1128,12 @@
       </c>
       <c r="G19" t="s">
         <v>23</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="L19" s="2"/>
     </row>
@@ -1002,8 +1141,9 @@
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C20">
         <v>16.436</v>
@@ -1020,14 +1160,21 @@
       <c r="G20" t="s">
         <v>23</v>
       </c>
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
-        <v>32</v>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C21">
         <v>16.536000000000001</v>
@@ -1049,8 +1196,9 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>30</v>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C22">
         <v>16.536000000000001</v>
@@ -1072,8 +1220,9 @@
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>32</v>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C23">
         <v>19.635999999999999</v>
@@ -1095,8 +1244,9 @@
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" t="s">
-        <v>30</v>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C24">
         <v>19.635999999999999</v>
@@ -1118,8 +1268,9 @@
       <c r="A25">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C25">
         <v>20.036000000000001</v>
@@ -1141,8 +1292,9 @@
       <c r="A26">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>30</v>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C26">
         <v>20.036000000000001</v>
@@ -1164,8 +1316,9 @@
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
-        <v>32</v>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C27">
         <v>20.436</v>
@@ -1187,8 +1340,9 @@
       <c r="A28">
         <v>2</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C28">
         <v>20.436</v>
@@ -1210,8 +1364,9 @@
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
-        <v>32</v>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C29">
         <v>20.835999999999999</v>
@@ -1233,8 +1388,9 @@
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C30">
         <v>20.835999999999999</v>
@@ -1256,8 +1412,9 @@
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C31">
         <v>21.236000000000001</v>
@@ -1279,8 +1436,9 @@
       <c r="A32">
         <v>3</v>
       </c>
-      <c r="B32" t="s">
-        <v>30</v>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C32">
         <v>35.636000000000003</v>
@@ -1302,8 +1460,9 @@
       <c r="A33">
         <v>3</v>
       </c>
-      <c r="B33" t="s">
-        <v>30</v>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C33">
         <v>36.036000000000001</v>
@@ -1325,8 +1484,9 @@
       <c r="A34">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
-        <v>30</v>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C34">
         <v>36.436</v>
@@ -1348,8 +1508,9 @@
       <c r="A35">
         <v>5</v>
       </c>
-      <c r="B35" t="s">
-        <v>30</v>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C35">
         <v>37.235999999999997</v>
@@ -1371,8 +1532,9 @@
       <c r="A36">
         <v>6</v>
       </c>
-      <c r="B36" t="s">
-        <v>30</v>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C36">
         <v>38.036000000000001</v>
@@ -1394,8 +1556,9 @@
       <c r="A37">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
-        <v>30</v>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C37">
         <v>38.835999999999999</v>
@@ -1417,8 +1580,9 @@
       <c r="A38">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
-        <v>30</v>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C38">
         <v>39.636000000000003</v>
@@ -1440,8 +1604,9 @@
       <c r="A39">
         <v>9</v>
       </c>
-      <c r="B39" t="s">
-        <v>30</v>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C39">
         <v>40.436</v>
@@ -1463,8 +1628,9 @@
       <c r="A40">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
-        <v>30</v>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C40">
         <v>41.235999999999997</v>
@@ -1486,8 +1652,9 @@
       <c r="A41">
         <v>11</v>
       </c>
-      <c r="B41" t="s">
-        <v>30</v>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C41">
         <v>42.036000000000001</v>
@@ -1509,8 +1676,9 @@
       <c r="A42">
         <v>12</v>
       </c>
-      <c r="B42" t="s">
-        <v>30</v>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C42">
         <v>42.835999999999999</v>
@@ -1532,8 +1700,9 @@
       <c r="A43">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
-        <v>30</v>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C43">
         <v>43.636000000000003</v>
@@ -1555,8 +1724,9 @@
       <c r="A44">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
-        <v>30</v>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C44">
         <v>44.436</v>
@@ -1578,8 +1748,9 @@
       <c r="A45">
         <v>15</v>
       </c>
-      <c r="B45" t="s">
-        <v>30</v>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C45">
         <v>45.235999999999997</v>
@@ -1601,8 +1772,9 @@
       <c r="A46">
         <v>16</v>
       </c>
-      <c r="B46" t="s">
-        <v>30</v>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C46">
         <v>46.036000000000001</v>
@@ -1624,8 +1796,9 @@
       <c r="A47">
         <v>1</v>
       </c>
-      <c r="B47" t="s">
-        <v>32</v>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C47">
         <v>72.635999999999996</v>
@@ -1647,8 +1820,9 @@
       <c r="A48">
         <v>3</v>
       </c>
-      <c r="B48" t="s">
-        <v>30</v>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C48">
         <v>72.635999999999996</v>
@@ -1670,8 +1844,9 @@
       <c r="A49">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
-        <v>32</v>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C49">
         <v>72.835999999999999</v>
@@ -1693,8 +1868,9 @@
       <c r="A50">
         <v>3</v>
       </c>
-      <c r="B50" t="s">
-        <v>30</v>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C50">
         <v>72.835999999999999</v>
@@ -1716,8 +1892,9 @@
       <c r="A51">
         <v>1</v>
       </c>
-      <c r="B51" t="s">
-        <v>32</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C51">
         <v>73.036000000000001</v>
@@ -1739,8 +1916,9 @@
       <c r="A52">
         <v>3</v>
       </c>
-      <c r="B52" t="s">
-        <v>30</v>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C52">
         <v>73.036000000000001</v>
@@ -1762,8 +1940,9 @@
       <c r="A53">
         <v>17</v>
       </c>
-      <c r="B53" t="s">
-        <v>30</v>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C53">
         <v>73.036000000000001</v>
@@ -1785,8 +1964,9 @@
       <c r="A54">
         <v>1</v>
       </c>
-      <c r="B54" t="s">
-        <v>32</v>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C54">
         <v>73.236000000000004</v>
@@ -1808,8 +1988,9 @@
       <c r="A55">
         <v>17</v>
       </c>
-      <c r="B55" t="s">
-        <v>30</v>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C55">
         <v>73.236000000000004</v>
@@ -1831,8 +2012,9 @@
       <c r="A56">
         <v>1</v>
       </c>
-      <c r="B56" t="s">
-        <v>32</v>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C56">
         <v>73.436000000000007</v>
@@ -1854,8 +2036,9 @@
       <c r="A57">
         <v>17</v>
       </c>
-      <c r="B57" t="s">
-        <v>30</v>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C57">
         <v>73.436000000000007</v>
@@ -1877,8 +2060,9 @@
       <c r="A58">
         <v>1</v>
       </c>
-      <c r="B58" t="s">
-        <v>32</v>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C58">
         <v>73.635999999999996</v>
@@ -1900,8 +2084,9 @@
       <c r="A59">
         <v>17</v>
       </c>
-      <c r="B59" t="s">
-        <v>30</v>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C59">
         <v>73.635999999999996</v>
@@ -1923,8 +2108,9 @@
       <c r="A60">
         <v>17</v>
       </c>
-      <c r="B60" t="s">
-        <v>30</v>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C60">
         <v>73.835999999999999</v>
@@ -1946,8 +2132,9 @@
       <c r="A61">
         <v>1</v>
       </c>
-      <c r="B61" t="s">
-        <v>32</v>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C61">
         <v>74.036000000000001</v>
@@ -1969,8 +2156,9 @@
       <c r="A62">
         <v>17</v>
       </c>
-      <c r="B62" t="s">
-        <v>30</v>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C62">
         <v>74.036000000000001</v>
@@ -1992,8 +2180,9 @@
       <c r="A63">
         <v>1</v>
       </c>
-      <c r="B63" t="s">
-        <v>32</v>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C63">
         <v>76.436000000000007</v>
@@ -2015,8 +2204,9 @@
       <c r="A64">
         <v>17</v>
       </c>
-      <c r="B64" t="s">
-        <v>30</v>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C64">
         <v>76.436000000000007</v>
@@ -2038,8 +2228,9 @@
       <c r="A65">
         <v>1</v>
       </c>
-      <c r="B65" t="s">
-        <v>32</v>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C65">
         <v>76.835999999999999</v>
@@ -2061,8 +2252,9 @@
       <c r="A66">
         <v>17</v>
       </c>
-      <c r="B66" t="s">
-        <v>30</v>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C66">
         <v>76.835999999999999</v>
@@ -2084,8 +2276,9 @@
       <c r="A67">
         <v>1</v>
       </c>
-      <c r="B67" t="s">
-        <v>32</v>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B130" si="1">VLOOKUP(A67,$I$1:$J$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C67">
         <v>77.236000000000004</v>
@@ -2107,8 +2300,9 @@
       <c r="A68">
         <v>17</v>
       </c>
-      <c r="B68" t="s">
-        <v>30</v>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C68">
         <v>77.236000000000004</v>
@@ -2130,8 +2324,9 @@
       <c r="A69">
         <v>1</v>
       </c>
-      <c r="B69" t="s">
-        <v>32</v>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C69">
         <v>82.835999999999999</v>
@@ -2153,8 +2348,9 @@
       <c r="A70">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>30</v>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C70">
         <v>82.835999999999999</v>
@@ -2176,8 +2372,9 @@
       <c r="A71">
         <v>1</v>
       </c>
-      <c r="B71" t="s">
-        <v>32</v>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C71">
         <v>83.236000000000004</v>
@@ -2199,8 +2396,9 @@
       <c r="A72">
         <v>17</v>
       </c>
-      <c r="B72" t="s">
-        <v>30</v>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C72">
         <v>83.236000000000004</v>
@@ -2222,8 +2420,9 @@
       <c r="A73">
         <v>1</v>
       </c>
-      <c r="B73" t="s">
-        <v>32</v>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C73">
         <v>83.635999999999996</v>
@@ -2245,8 +2444,9 @@
       <c r="A74">
         <v>17</v>
       </c>
-      <c r="B74" t="s">
-        <v>30</v>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C74">
         <v>83.635999999999996</v>
@@ -2268,8 +2468,9 @@
       <c r="A75">
         <v>17</v>
       </c>
-      <c r="B75" t="s">
-        <v>30</v>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C75">
         <v>85.236000000000004</v>
@@ -2291,8 +2492,9 @@
       <c r="A76">
         <v>1</v>
       </c>
-      <c r="B76" t="s">
-        <v>32</v>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C76">
         <v>86.036000000000001</v>
@@ -2314,8 +2516,9 @@
       <c r="A77">
         <v>17</v>
       </c>
-      <c r="B77" t="s">
-        <v>30</v>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C77">
         <v>86.036000000000001</v>
@@ -2337,8 +2540,9 @@
       <c r="A78">
         <v>1</v>
       </c>
-      <c r="B78" t="s">
-        <v>32</v>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C78">
         <v>86.436000000000007</v>
@@ -2360,8 +2564,9 @@
       <c r="A79">
         <v>1</v>
       </c>
-      <c r="B79" t="s">
-        <v>32</v>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C79">
         <v>86.835999999999999</v>
@@ -2383,8 +2588,9 @@
       <c r="A80">
         <v>17</v>
       </c>
-      <c r="B80" t="s">
-        <v>30</v>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C80">
         <v>86.436000000000007</v>
@@ -2406,8 +2612,9 @@
       <c r="A81">
         <v>1</v>
       </c>
-      <c r="B81" t="s">
-        <v>32</v>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C81">
         <v>89.236000000000004</v>
@@ -2429,8 +2636,9 @@
       <c r="A82">
         <v>17</v>
       </c>
-      <c r="B82" t="s">
-        <v>30</v>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C82">
         <v>89.236000000000004</v>
@@ -2452,8 +2660,9 @@
       <c r="A83">
         <v>1</v>
       </c>
-      <c r="B83" t="s">
-        <v>32</v>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C83">
         <v>89.635999999999996</v>
@@ -2475,8 +2684,9 @@
       <c r="A84">
         <v>17</v>
       </c>
-      <c r="B84" t="s">
-        <v>30</v>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C84">
         <v>89.635999999999996</v>
@@ -2498,8 +2708,9 @@
       <c r="A85">
         <v>1</v>
       </c>
-      <c r="B85" t="s">
-        <v>32</v>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C85">
         <v>90.036000000000001</v>
@@ -2521,8 +2732,9 @@
       <c r="A86">
         <v>17</v>
       </c>
-      <c r="B86" t="s">
-        <v>30</v>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C86">
         <v>90.036000000000001</v>
@@ -2544,8 +2756,9 @@
       <c r="A87">
         <v>1</v>
       </c>
-      <c r="B87" t="s">
-        <v>32</v>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C87">
         <v>95.63600000000001</v>
@@ -2567,8 +2780,9 @@
       <c r="A88">
         <v>17</v>
       </c>
-      <c r="B88" t="s">
-        <v>30</v>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C88">
         <v>95.63600000000001</v>
@@ -2590,8 +2804,9 @@
       <c r="A89">
         <v>1</v>
       </c>
-      <c r="B89" t="s">
-        <v>32</v>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C89">
         <v>96.036000000000001</v>
@@ -2613,8 +2828,9 @@
       <c r="A90">
         <v>17</v>
       </c>
-      <c r="B90" t="s">
-        <v>30</v>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C90">
         <v>96.036000000000001</v>
@@ -2636,8 +2852,9 @@
       <c r="A91">
         <v>1</v>
       </c>
-      <c r="B91" t="s">
-        <v>32</v>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C91">
         <v>96.436000000000007</v>
@@ -2659,8 +2876,9 @@
       <c r="A92">
         <v>17</v>
       </c>
-      <c r="B92" t="s">
-        <v>30</v>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C92">
         <v>96.436000000000007</v>
@@ -2682,8 +2900,9 @@
       <c r="A93">
         <v>1</v>
       </c>
-      <c r="B93" t="s">
-        <v>32</v>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C93">
         <v>97.236000000000004</v>
@@ -2705,8 +2924,9 @@
       <c r="A94">
         <v>17</v>
       </c>
-      <c r="B94" t="s">
-        <v>30</v>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C94">
         <v>97.236000000000004</v>
@@ -2728,8 +2948,9 @@
       <c r="A95">
         <v>1</v>
       </c>
-      <c r="B95" t="s">
-        <v>32</v>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C95">
         <v>97.536000000000001</v>
@@ -2751,8 +2972,9 @@
       <c r="A96">
         <v>17</v>
       </c>
-      <c r="B96" t="s">
-        <v>30</v>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C96">
         <v>97.536000000000001</v>
@@ -2774,8 +2996,9 @@
       <c r="A97">
         <v>1</v>
       </c>
-      <c r="B97" t="s">
-        <v>32</v>
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C97">
         <v>97.835999999999999</v>
@@ -2797,8 +3020,9 @@
       <c r="A98">
         <v>17</v>
       </c>
-      <c r="B98" t="s">
-        <v>30</v>
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C98">
         <v>97.835999999999999</v>
@@ -2820,8 +3044,9 @@
       <c r="A99">
         <v>1</v>
       </c>
-      <c r="B99" t="s">
-        <v>32</v>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C99">
         <v>98.135999999999996</v>
@@ -2843,8 +3068,9 @@
       <c r="A100">
         <v>17</v>
       </c>
-      <c r="B100" t="s">
-        <v>30</v>
+      <c r="B100" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C100">
         <v>98.135999999999996</v>
@@ -2866,8 +3092,9 @@
       <c r="A101">
         <v>1</v>
       </c>
-      <c r="B101" t="s">
-        <v>32</v>
+      <c r="B101" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C101">
         <v>98.835999999999999</v>
@@ -2889,8 +3116,9 @@
       <c r="A102">
         <v>1</v>
       </c>
-      <c r="B102" t="s">
-        <v>32</v>
+      <c r="B102" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C102">
         <v>99.034999999999997</v>
@@ -2912,8 +3140,9 @@
       <c r="A103">
         <v>1</v>
       </c>
-      <c r="B103" t="s">
-        <v>32</v>
+      <c r="B103" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C103">
         <v>99.036000000000001</v>
@@ -2935,8 +3164,9 @@
       <c r="A104">
         <v>1</v>
       </c>
-      <c r="B104" t="s">
-        <v>32</v>
+      <c r="B104" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C104">
         <v>99.234999999999999</v>
@@ -2958,8 +3188,9 @@
       <c r="A105">
         <v>1</v>
       </c>
-      <c r="B105" t="s">
-        <v>32</v>
+      <c r="B105" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C105">
         <v>99.236000000000004</v>
@@ -2981,8 +3212,9 @@
       <c r="A106">
         <v>1</v>
       </c>
-      <c r="B106" t="s">
-        <v>32</v>
+      <c r="B106" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C106">
         <v>99.435000000000002</v>
@@ -3004,8 +3236,9 @@
       <c r="A107">
         <v>1</v>
       </c>
-      <c r="B107" t="s">
-        <v>32</v>
+      <c r="B107" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C107">
         <v>99.436000000000007</v>
@@ -3027,8 +3260,9 @@
       <c r="A108">
         <v>17</v>
       </c>
-      <c r="B108" t="s">
-        <v>30</v>
+      <c r="B108" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C108">
         <v>98.835999999999999</v>
@@ -3050,8 +3284,9 @@
       <c r="A109">
         <v>1</v>
       </c>
-      <c r="B109" t="s">
-        <v>32</v>
+      <c r="B109" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C109">
         <v>99.635999999999996</v>
@@ -3073,8 +3308,9 @@
       <c r="A110">
         <v>17</v>
       </c>
-      <c r="B110" t="s">
-        <v>30</v>
+      <c r="B110" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C110">
         <v>99.635999999999996</v>
@@ -3096,8 +3332,9 @@
       <c r="A111">
         <v>1</v>
       </c>
-      <c r="B111" t="s">
-        <v>32</v>
+      <c r="B111" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C111">
         <v>99.736000000000004</v>
@@ -3119,8 +3356,9 @@
       <c r="A112">
         <v>17</v>
       </c>
-      <c r="B112" t="s">
-        <v>30</v>
+      <c r="B112" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C112">
         <v>99.736000000000004</v>
@@ -3142,8 +3380,9 @@
       <c r="A113">
         <v>17</v>
       </c>
-      <c r="B113" t="s">
-        <v>30</v>
+      <c r="B113" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C113">
         <v>108.43600000000001</v>
@@ -3165,8 +3404,9 @@
       <c r="A114">
         <v>1</v>
       </c>
-      <c r="B114" t="s">
-        <v>32</v>
+      <c r="B114" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C114">
         <v>109.236</v>
@@ -3188,8 +3428,9 @@
       <c r="A115">
         <v>1</v>
       </c>
-      <c r="B115" t="s">
-        <v>32</v>
+      <c r="B115" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C115">
         <v>109.336</v>
@@ -3211,8 +3452,9 @@
       <c r="A116">
         <v>17</v>
       </c>
-      <c r="B116" t="s">
-        <v>30</v>
+      <c r="B116" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C116">
         <v>109.236</v>
@@ -3234,8 +3476,9 @@
       <c r="A117">
         <v>17</v>
       </c>
-      <c r="B117" t="s">
-        <v>30</v>
+      <c r="B117" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C117">
         <v>110.83600000000001</v>
@@ -3257,8 +3500,9 @@
       <c r="A118">
         <v>1</v>
       </c>
-      <c r="B118" t="s">
-        <v>32</v>
+      <c r="B118" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C118">
         <v>111.636</v>
@@ -3280,8 +3524,9 @@
       <c r="A119">
         <v>17</v>
       </c>
-      <c r="B119" t="s">
-        <v>30</v>
+      <c r="B119" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C119">
         <v>111.636</v>
@@ -3303,8 +3548,9 @@
       <c r="A120">
         <v>1</v>
       </c>
-      <c r="B120" t="s">
-        <v>32</v>
+      <c r="B120" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C120">
         <v>112.036</v>
@@ -3326,8 +3572,9 @@
       <c r="A121">
         <v>1</v>
       </c>
-      <c r="B121" t="s">
-        <v>32</v>
+      <c r="B121" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C121">
         <v>112.43600000000001</v>
@@ -3349,8 +3596,9 @@
       <c r="A122">
         <v>17</v>
       </c>
-      <c r="B122" t="s">
-        <v>30</v>
+      <c r="B122" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C122">
         <v>112.036</v>
@@ -3372,8 +3620,9 @@
       <c r="A123">
         <v>1</v>
       </c>
-      <c r="B123" t="s">
-        <v>32</v>
+      <c r="B123" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C123">
         <v>121.236</v>
@@ -3395,8 +3644,9 @@
       <c r="A124">
         <v>1</v>
       </c>
-      <c r="B124" t="s">
-        <v>32</v>
+      <c r="B124" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C124">
         <v>122.036</v>
@@ -3418,8 +3668,9 @@
       <c r="A125">
         <v>1</v>
       </c>
-      <c r="B125" t="s">
-        <v>32</v>
+      <c r="B125" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C125">
         <v>122.43600000000001</v>
@@ -3441,8 +3692,9 @@
       <c r="A126">
         <v>17</v>
       </c>
-      <c r="B126" t="s">
-        <v>30</v>
+      <c r="B126" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C126">
         <v>123.652</v>
@@ -3464,8 +3716,9 @@
       <c r="A127">
         <v>17</v>
       </c>
-      <c r="B127" t="s">
-        <v>30</v>
+      <c r="B127" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C127">
         <v>125.152</v>
@@ -3487,8 +3740,9 @@
       <c r="A128">
         <v>17</v>
       </c>
-      <c r="B128" t="s">
-        <v>30</v>
+      <c r="B128" t="str">
+        <f t="shared" si="1"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C128">
         <v>125.97199999999999</v>
@@ -3510,8 +3764,9 @@
       <c r="A129">
         <v>18</v>
       </c>
-      <c r="B129" t="s">
-        <v>31</v>
+      <c r="B129" t="str">
+        <f t="shared" si="1"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C129">
         <v>125.152</v>
@@ -3533,8 +3788,9 @@
       <c r="A130">
         <v>18</v>
       </c>
-      <c r="B130" t="s">
-        <v>31</v>
+      <c r="B130" t="str">
+        <f t="shared" si="1"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C130">
         <v>125.97199999999999</v>
@@ -3556,8 +3812,9 @@
       <c r="A131">
         <v>17</v>
       </c>
-      <c r="B131" t="s">
-        <v>30</v>
+      <c r="B131" t="str">
+        <f t="shared" ref="B131:B194" si="2">VLOOKUP(A131,$I$1:$J$20,2,FALSE)</f>
+        <v>#f0ffff</v>
       </c>
       <c r="C131">
         <v>128.447</v>
@@ -3579,8 +3836,9 @@
       <c r="A132">
         <v>17</v>
       </c>
-      <c r="B132" t="s">
-        <v>30</v>
+      <c r="B132" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C132">
         <v>129.267</v>
@@ -3602,8 +3860,9 @@
       <c r="A133">
         <v>18</v>
       </c>
-      <c r="B133" t="s">
-        <v>31</v>
+      <c r="B133" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C133">
         <v>128.447</v>
@@ -3625,8 +3884,9 @@
       <c r="A134">
         <v>18</v>
       </c>
-      <c r="B134" t="s">
-        <v>31</v>
+      <c r="B134" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C134">
         <v>129.267</v>
@@ -3648,8 +3908,9 @@
       <c r="A135">
         <v>17</v>
       </c>
-      <c r="B135" t="s">
-        <v>30</v>
+      <c r="B135" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C135">
         <v>131.637</v>
@@ -3671,8 +3932,9 @@
       <c r="A136">
         <v>17</v>
       </c>
-      <c r="B136" t="s">
-        <v>30</v>
+      <c r="B136" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C136">
         <v>132.45699999999999</v>
@@ -3694,8 +3956,9 @@
       <c r="A137">
         <v>18</v>
       </c>
-      <c r="B137" t="s">
-        <v>31</v>
+      <c r="B137" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C137">
         <v>131.637</v>
@@ -3717,8 +3980,9 @@
       <c r="A138">
         <v>18</v>
       </c>
-      <c r="B138" t="s">
-        <v>31</v>
+      <c r="B138" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C138">
         <v>132.45699999999999</v>
@@ -3740,8 +4004,9 @@
       <c r="A139">
         <v>17</v>
       </c>
-      <c r="B139" t="s">
-        <v>30</v>
+      <c r="B139" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C139">
         <v>134.83600000000001</v>
@@ -3763,8 +4028,9 @@
       <c r="A140">
         <v>17</v>
       </c>
-      <c r="B140" t="s">
-        <v>30</v>
+      <c r="B140" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C140">
         <v>135.43600000000004</v>
@@ -3786,8 +4052,9 @@
       <c r="A141">
         <v>17</v>
       </c>
-      <c r="B141" t="s">
-        <v>30</v>
+      <c r="B141" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C141">
         <v>136.03600000000006</v>
@@ -3809,8 +4076,9 @@
       <c r="A142">
         <v>1</v>
       </c>
-      <c r="B142" t="s">
-        <v>32</v>
+      <c r="B142" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C142">
         <v>137.636</v>
@@ -3832,8 +4100,9 @@
       <c r="A143">
         <v>1</v>
       </c>
-      <c r="B143" t="s">
-        <v>32</v>
+      <c r="B143" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C143">
         <v>138.036</v>
@@ -3855,8 +4124,9 @@
       <c r="A144">
         <v>1</v>
       </c>
-      <c r="B144" t="s">
-        <v>32</v>
+      <c r="B144" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C144">
         <v>138.23599999999999</v>
@@ -3878,8 +4148,9 @@
       <c r="A145">
         <v>1</v>
       </c>
-      <c r="B145" t="s">
-        <v>32</v>
+      <c r="B145" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C145">
         <v>138.636</v>
@@ -3901,8 +4172,9 @@
       <c r="A146">
         <v>17</v>
       </c>
-      <c r="B146" t="s">
-        <v>30</v>
+      <c r="B146" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C146">
         <v>141.23599999999999</v>
@@ -3924,8 +4196,9 @@
       <c r="A147">
         <v>1</v>
       </c>
-      <c r="B147" t="s">
-        <v>32</v>
+      <c r="B147" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C147">
         <v>141.23599999999999</v>
@@ -3947,8 +4220,9 @@
       <c r="A148">
         <v>17</v>
       </c>
-      <c r="B148" t="s">
-        <v>30</v>
+      <c r="B148" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C148">
         <v>141.636</v>
@@ -3970,8 +4244,9 @@
       <c r="A149">
         <v>1</v>
       </c>
-      <c r="B149" t="s">
-        <v>32</v>
+      <c r="B149" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C149">
         <v>141.636</v>
@@ -3993,8 +4268,9 @@
       <c r="A150">
         <v>1</v>
       </c>
-      <c r="B150" t="s">
-        <v>32</v>
+      <c r="B150" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C150">
         <v>151.036</v>
@@ -4016,8 +4292,9 @@
       <c r="A151">
         <v>1</v>
       </c>
-      <c r="B151" t="s">
-        <v>32</v>
+      <c r="B151" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C151">
         <v>151.43600000000001</v>
@@ -4039,8 +4316,9 @@
       <c r="A152">
         <v>1</v>
       </c>
-      <c r="B152" t="s">
-        <v>32</v>
+      <c r="B152" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C152">
         <v>152.036</v>
@@ -4062,8 +4340,9 @@
       <c r="A153">
         <v>1</v>
       </c>
-      <c r="B153" t="s">
-        <v>32</v>
+      <c r="B153" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C153">
         <v>152.23599999999999</v>
@@ -4085,8 +4364,9 @@
       <c r="A154">
         <v>17</v>
       </c>
-      <c r="B154" t="s">
-        <v>30</v>
+      <c r="B154" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C154">
         <v>151.036</v>
@@ -4108,8 +4388,9 @@
       <c r="A155">
         <v>17</v>
       </c>
-      <c r="B155" t="s">
-        <v>30</v>
+      <c r="B155" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C155">
         <v>151.43600000000001</v>
@@ -4131,8 +4412,9 @@
       <c r="A156">
         <v>17</v>
       </c>
-      <c r="B156" t="s">
-        <v>30</v>
+      <c r="B156" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C156">
         <v>152.036</v>
@@ -4154,8 +4436,9 @@
       <c r="A157">
         <v>17</v>
       </c>
-      <c r="B157" t="s">
-        <v>30</v>
+      <c r="B157" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C157">
         <v>152.23599999999999</v>
@@ -4177,8 +4460,9 @@
       <c r="A158">
         <v>1</v>
       </c>
-      <c r="B158" t="s">
-        <v>32</v>
+      <c r="B158" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C158">
         <v>161.636</v>
@@ -4200,8 +4484,9 @@
       <c r="A159">
         <v>1</v>
       </c>
-      <c r="B159" t="s">
-        <v>32</v>
+      <c r="B159" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C159">
         <v>161.83600000000001</v>
@@ -4223,8 +4508,9 @@
       <c r="A160">
         <v>1</v>
       </c>
-      <c r="B160" t="s">
-        <v>32</v>
+      <c r="B160" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C160">
         <v>163.636</v>
@@ -4246,8 +4532,9 @@
       <c r="A161">
         <v>1</v>
       </c>
-      <c r="B161" t="s">
-        <v>32</v>
+      <c r="B161" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C161">
         <v>168.43600000000001</v>
@@ -4269,8 +4556,9 @@
       <c r="A162">
         <v>1</v>
       </c>
-      <c r="B162" t="s">
-        <v>32</v>
+      <c r="B162" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C162">
         <v>170.036</v>
@@ -4292,8 +4580,9 @@
       <c r="A163">
         <v>1</v>
       </c>
-      <c r="B163" t="s">
-        <v>32</v>
+      <c r="B163" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C163">
         <v>172.83600000000001</v>
@@ -4315,8 +4604,9 @@
       <c r="A164">
         <v>1</v>
       </c>
-      <c r="B164" t="s">
-        <v>32</v>
+      <c r="B164" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C164">
         <v>173.23599999999999</v>
@@ -4338,8 +4628,9 @@
       <c r="A165">
         <v>17</v>
       </c>
-      <c r="B165" t="s">
-        <v>30</v>
+      <c r="B165" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C165">
         <v>187.83600000000001</v>
@@ -4361,8 +4652,9 @@
       <c r="A166">
         <v>1</v>
       </c>
-      <c r="B166" t="s">
-        <v>32</v>
+      <c r="B166" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C166">
         <v>187.83600000000001</v>
@@ -4384,8 +4676,9 @@
       <c r="A167">
         <v>17</v>
       </c>
-      <c r="B167" t="s">
-        <v>30</v>
+      <c r="B167" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C167">
         <v>188.036</v>
@@ -4407,8 +4700,9 @@
       <c r="A168">
         <v>1</v>
       </c>
-      <c r="B168" t="s">
-        <v>32</v>
+      <c r="B168" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C168">
         <v>188.036</v>
@@ -4430,8 +4724,9 @@
       <c r="A169">
         <v>17</v>
       </c>
-      <c r="B169" t="s">
-        <v>30</v>
+      <c r="B169" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C169">
         <v>188.23599999999999</v>
@@ -4453,8 +4748,9 @@
       <c r="A170">
         <v>1</v>
       </c>
-      <c r="B170" t="s">
-        <v>32</v>
+      <c r="B170" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C170">
         <v>188.23599999999999</v>
@@ -4476,8 +4772,9 @@
       <c r="A171">
         <v>19</v>
       </c>
-      <c r="B171" t="s">
-        <v>32</v>
+      <c r="B171" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C171">
         <v>188.23599999999999</v>
@@ -4499,8 +4796,9 @@
       <c r="A172">
         <v>17</v>
       </c>
-      <c r="B172" t="s">
-        <v>30</v>
+      <c r="B172" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C172">
         <v>188.43600000000001</v>
@@ -4522,8 +4820,9 @@
       <c r="A173">
         <v>19</v>
       </c>
-      <c r="B173" t="s">
-        <v>32</v>
+      <c r="B173" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C173">
         <v>188.43600000000001</v>
@@ -4545,8 +4844,9 @@
       <c r="A174">
         <v>17</v>
       </c>
-      <c r="B174" t="s">
-        <v>30</v>
+      <c r="B174" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C174">
         <v>188.63600000000002</v>
@@ -4568,8 +4868,9 @@
       <c r="A175">
         <v>19</v>
       </c>
-      <c r="B175" t="s">
-        <v>32</v>
+      <c r="B175" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C175">
         <v>188.63600000000002</v>
@@ -4591,8 +4892,9 @@
       <c r="A176">
         <v>17</v>
       </c>
-      <c r="B176" t="s">
-        <v>30</v>
+      <c r="B176" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C176">
         <v>188.83600000000001</v>
@@ -4614,8 +4916,9 @@
       <c r="A177">
         <v>19</v>
       </c>
-      <c r="B177" t="s">
-        <v>32</v>
+      <c r="B177" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C177">
         <v>188.83600000000001</v>
@@ -4637,8 +4940,9 @@
       <c r="A178">
         <v>19</v>
       </c>
-      <c r="B178" t="s">
-        <v>32</v>
+      <c r="B178" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C178">
         <v>189.036</v>
@@ -4660,8 +4964,9 @@
       <c r="A179">
         <v>17</v>
       </c>
-      <c r="B179" t="s">
-        <v>30</v>
+      <c r="B179" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C179">
         <v>189.23599999999999</v>
@@ -4683,8 +4988,9 @@
       <c r="A180">
         <v>19</v>
       </c>
-      <c r="B180" t="s">
-        <v>32</v>
+      <c r="B180" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C180">
         <v>189.23599999999999</v>
@@ -4706,8 +5012,9 @@
       <c r="A181">
         <v>17</v>
       </c>
-      <c r="B181" t="s">
-        <v>30</v>
+      <c r="B181" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C181">
         <v>194.83600000000001</v>
@@ -4729,8 +5036,9 @@
       <c r="A182">
         <v>19</v>
       </c>
-      <c r="B182" t="s">
-        <v>32</v>
+      <c r="B182" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C182">
         <v>194.83600000000001</v>
@@ -4752,8 +5060,9 @@
       <c r="A183">
         <v>17</v>
       </c>
-      <c r="B183" t="s">
-        <v>30</v>
+      <c r="B183" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C183">
         <v>195.136</v>
@@ -4775,8 +5084,9 @@
       <c r="A184">
         <v>19</v>
       </c>
-      <c r="B184" t="s">
-        <v>32</v>
+      <c r="B184" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C184">
         <v>195.136</v>
@@ -4798,8 +5108,9 @@
       <c r="A185">
         <v>17</v>
       </c>
-      <c r="B185" t="s">
-        <v>30</v>
+      <c r="B185" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C185">
         <v>195.43600000000001</v>
@@ -4821,8 +5132,9 @@
       <c r="A186">
         <v>19</v>
       </c>
-      <c r="B186" t="s">
-        <v>32</v>
+      <c r="B186" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C186">
         <v>195.43600000000001</v>
@@ -4844,8 +5156,9 @@
       <c r="A187">
         <v>17</v>
       </c>
-      <c r="B187" t="s">
-        <v>30</v>
+      <c r="B187" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C187">
         <v>195.636</v>
@@ -4867,8 +5180,9 @@
       <c r="A188">
         <v>19</v>
       </c>
-      <c r="B188" t="s">
-        <v>32</v>
+      <c r="B188" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C188">
         <v>195.636</v>
@@ -4890,8 +5204,9 @@
       <c r="A189">
         <v>17</v>
       </c>
-      <c r="B189" t="s">
-        <v>30</v>
+      <c r="B189" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C189">
         <v>195.93600000000001</v>
@@ -4913,8 +5228,9 @@
       <c r="A190">
         <v>19</v>
       </c>
-      <c r="B190" t="s">
-        <v>32</v>
+      <c r="B190" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C190">
         <v>195.93600000000001</v>
@@ -4936,8 +5252,9 @@
       <c r="A191">
         <v>17</v>
       </c>
-      <c r="B191" t="s">
-        <v>30</v>
+      <c r="B191" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C191">
         <v>196.23599999999999</v>
@@ -4959,8 +5276,9 @@
       <c r="A192">
         <v>19</v>
       </c>
-      <c r="B192" t="s">
-        <v>32</v>
+      <c r="B192" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C192">
         <v>196.23599999999999</v>
@@ -4982,8 +5300,9 @@
       <c r="A193">
         <v>17</v>
       </c>
-      <c r="B193" t="s">
-        <v>30</v>
+      <c r="B193" t="str">
+        <f t="shared" si="2"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C193">
         <v>196.43600000000001</v>
@@ -5005,8 +5324,9 @@
       <c r="A194">
         <v>19</v>
       </c>
-      <c r="B194" t="s">
-        <v>32</v>
+      <c r="B194" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C194">
         <v>196.43600000000001</v>
@@ -5028,8 +5348,9 @@
       <c r="A195">
         <v>17</v>
       </c>
-      <c r="B195" t="s">
-        <v>30</v>
+      <c r="B195" t="str">
+        <f t="shared" ref="B195:B240" si="3">VLOOKUP(A195,$I$1:$J$20,2,FALSE)</f>
+        <v>#f0ffff</v>
       </c>
       <c r="C195">
         <v>200.23599999999999</v>
@@ -5051,8 +5372,9 @@
       <c r="A196">
         <v>17</v>
       </c>
-      <c r="B196" t="s">
-        <v>30</v>
+      <c r="B196" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C196">
         <v>200.83600000000001</v>
@@ -5074,8 +5396,9 @@
       <c r="A197">
         <v>19</v>
       </c>
-      <c r="B197" t="s">
-        <v>32</v>
+      <c r="B197" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C197">
         <v>201.636</v>
@@ -5097,8 +5420,9 @@
       <c r="A198">
         <v>19</v>
       </c>
-      <c r="B198" t="s">
-        <v>32</v>
+      <c r="B198" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C198">
         <v>201.73599999999999</v>
@@ -5120,8 +5444,9 @@
       <c r="A199">
         <v>17</v>
       </c>
-      <c r="B199" t="s">
-        <v>30</v>
+      <c r="B199" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C199">
         <v>207.63600000000002</v>
@@ -5143,8 +5468,9 @@
       <c r="A200">
         <v>19</v>
       </c>
-      <c r="B200" t="s">
-        <v>32</v>
+      <c r="B200" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C200">
         <v>207.63600000000002</v>
@@ -5166,8 +5492,9 @@
       <c r="A201">
         <v>17</v>
       </c>
-      <c r="B201" t="s">
-        <v>30</v>
+      <c r="B201" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C201">
         <v>207.93600000000001</v>
@@ -5189,8 +5516,9 @@
       <c r="A202">
         <v>19</v>
       </c>
-      <c r="B202" t="s">
-        <v>32</v>
+      <c r="B202" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C202">
         <v>207.93600000000001</v>
@@ -5212,8 +5540,9 @@
       <c r="A203">
         <v>17</v>
       </c>
-      <c r="B203" t="s">
-        <v>30</v>
+      <c r="B203" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C203">
         <v>208.23600000000002</v>
@@ -5235,8 +5564,9 @@
       <c r="A204">
         <v>19</v>
       </c>
-      <c r="B204" t="s">
-        <v>32</v>
+      <c r="B204" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C204">
         <v>208.23600000000002</v>
@@ -5258,8 +5588,9 @@
       <c r="A205">
         <v>17</v>
       </c>
-      <c r="B205" t="s">
-        <v>30</v>
+      <c r="B205" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C205">
         <v>208.43600000000001</v>
@@ -5281,8 +5612,9 @@
       <c r="A206">
         <v>19</v>
       </c>
-      <c r="B206" t="s">
-        <v>32</v>
+      <c r="B206" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C206">
         <v>208.43600000000001</v>
@@ -5304,8 +5636,9 @@
       <c r="A207">
         <v>17</v>
       </c>
-      <c r="B207" t="s">
-        <v>30</v>
+      <c r="B207" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C207">
         <v>208.73600000000002</v>
@@ -5327,8 +5660,9 @@
       <c r="A208">
         <v>19</v>
       </c>
-      <c r="B208" t="s">
-        <v>32</v>
+      <c r="B208" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C208">
         <v>208.73600000000002</v>
@@ -5350,8 +5684,9 @@
       <c r="A209">
         <v>17</v>
       </c>
-      <c r="B209" t="s">
-        <v>30</v>
+      <c r="B209" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C209">
         <v>209.036</v>
@@ -5373,8 +5708,9 @@
       <c r="A210">
         <v>19</v>
       </c>
-      <c r="B210" t="s">
-        <v>32</v>
+      <c r="B210" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C210">
         <v>209.036</v>
@@ -5396,8 +5732,9 @@
       <c r="A211">
         <v>17</v>
       </c>
-      <c r="B211" t="s">
-        <v>30</v>
+      <c r="B211" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C211">
         <v>209.23600000000002</v>
@@ -5419,8 +5756,9 @@
       <c r="A212">
         <v>19</v>
       </c>
-      <c r="B212" t="s">
-        <v>32</v>
+      <c r="B212" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C212">
         <v>209.23600000000002</v>
@@ -5442,8 +5780,9 @@
       <c r="A213">
         <v>17</v>
       </c>
-      <c r="B213" t="s">
-        <v>30</v>
+      <c r="B213" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C213">
         <v>219.23599999999999</v>
@@ -5465,8 +5804,9 @@
       <c r="A214">
         <v>19</v>
       </c>
-      <c r="B214" t="s">
-        <v>32</v>
+      <c r="B214" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C214">
         <v>219.23599999999999</v>
@@ -5488,8 +5828,9 @@
       <c r="A215">
         <v>17</v>
       </c>
-      <c r="B215" t="s">
-        <v>30</v>
+      <c r="B215" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C215">
         <v>219.536</v>
@@ -5511,8 +5852,9 @@
       <c r="A216">
         <v>19</v>
       </c>
-      <c r="B216" t="s">
-        <v>32</v>
+      <c r="B216" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C216">
         <v>219.536</v>
@@ -5534,8 +5876,9 @@
       <c r="A217">
         <v>17</v>
       </c>
-      <c r="B217" t="s">
-        <v>30</v>
+      <c r="B217" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C217">
         <v>219.83600000000001</v>
@@ -5557,8 +5900,9 @@
       <c r="A218">
         <v>19</v>
       </c>
-      <c r="B218" t="s">
-        <v>32</v>
+      <c r="B218" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C218">
         <v>219.83600000000001</v>
@@ -5580,8 +5924,9 @@
       <c r="A219">
         <v>17</v>
       </c>
-      <c r="B219" t="s">
-        <v>30</v>
+      <c r="B219" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C219">
         <v>220.136</v>
@@ -5603,8 +5948,9 @@
       <c r="A220">
         <v>19</v>
       </c>
-      <c r="B220" t="s">
-        <v>32</v>
+      <c r="B220" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C220">
         <v>220.136</v>
@@ -5626,8 +5972,9 @@
       <c r="A221">
         <v>17</v>
       </c>
-      <c r="B221" t="s">
-        <v>30</v>
+      <c r="B221" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C221">
         <v>220.43600000000001</v>
@@ -5649,8 +5996,9 @@
       <c r="A222">
         <v>19</v>
       </c>
-      <c r="B222" t="s">
-        <v>32</v>
+      <c r="B222" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C222">
         <v>220.43600000000001</v>
@@ -5672,8 +6020,9 @@
       <c r="A223">
         <v>17</v>
       </c>
-      <c r="B223" t="s">
-        <v>30</v>
+      <c r="B223" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C223">
         <v>232.036</v>
@@ -5695,8 +6044,9 @@
       <c r="A224">
         <v>19</v>
       </c>
-      <c r="B224" t="s">
-        <v>32</v>
+      <c r="B224" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C224">
         <v>232.036</v>
@@ -5718,8 +6068,9 @@
       <c r="A225">
         <v>17</v>
       </c>
-      <c r="B225" t="s">
-        <v>30</v>
+      <c r="B225" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C225">
         <v>232.33600000000001</v>
@@ -5741,8 +6092,9 @@
       <c r="A226">
         <v>19</v>
       </c>
-      <c r="B226" t="s">
-        <v>32</v>
+      <c r="B226" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C226">
         <v>232.33600000000001</v>
@@ -5764,8 +6116,9 @@
       <c r="A227">
         <v>17</v>
       </c>
-      <c r="B227" t="s">
-        <v>30</v>
+      <c r="B227" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C227">
         <v>232.63600000000002</v>
@@ -5787,8 +6140,9 @@
       <c r="A228">
         <v>19</v>
       </c>
-      <c r="B228" t="s">
-        <v>32</v>
+      <c r="B228" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C228">
         <v>232.63600000000002</v>
@@ -5810,8 +6164,9 @@
       <c r="A229">
         <v>17</v>
       </c>
-      <c r="B229" t="s">
-        <v>30</v>
+      <c r="B229" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C229">
         <v>232.93600000000001</v>
@@ -5833,8 +6188,9 @@
       <c r="A230">
         <v>19</v>
       </c>
-      <c r="B230" t="s">
-        <v>32</v>
+      <c r="B230" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C230">
         <v>232.93600000000001</v>
@@ -5856,8 +6212,9 @@
       <c r="A231">
         <v>17</v>
       </c>
-      <c r="B231" t="s">
-        <v>30</v>
+      <c r="B231" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C231">
         <v>233.23600000000002</v>
@@ -5879,8 +6236,9 @@
       <c r="A232">
         <v>19</v>
       </c>
-      <c r="B232" t="s">
-        <v>32</v>
+      <c r="B232" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C232">
         <v>233.23600000000002</v>
@@ -5902,8 +6260,9 @@
       <c r="A233">
         <v>17</v>
       </c>
-      <c r="B233" t="s">
-        <v>30</v>
+      <c r="B233" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C233">
         <v>238.43600000000001</v>
@@ -5925,8 +6284,9 @@
       <c r="A234">
         <v>19</v>
       </c>
-      <c r="B234" t="s">
-        <v>32</v>
+      <c r="B234" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C234">
         <v>238.43600000000001</v>
@@ -5948,8 +6308,9 @@
       <c r="A235">
         <v>17</v>
       </c>
-      <c r="B235" t="s">
-        <v>30</v>
+      <c r="B235" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C235">
         <v>238.83600000000001</v>
@@ -5971,8 +6332,9 @@
       <c r="A236">
         <v>19</v>
       </c>
-      <c r="B236" t="s">
-        <v>32</v>
+      <c r="B236" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C236">
         <v>238.83600000000001</v>
@@ -5994,8 +6356,9 @@
       <c r="A237">
         <v>17</v>
       </c>
-      <c r="B237" t="s">
-        <v>30</v>
+      <c r="B237" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C237">
         <v>240.43600000000001</v>
@@ -6017,8 +6380,9 @@
       <c r="A238">
         <v>19</v>
       </c>
-      <c r="B238" t="s">
-        <v>32</v>
+      <c r="B238" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C238">
         <v>240.43600000000001</v>
@@ -6040,8 +6404,9 @@
       <c r="A239">
         <v>17</v>
       </c>
-      <c r="B239" t="s">
-        <v>30</v>
+      <c r="B239" t="str">
+        <f t="shared" si="3"/>
+        <v>#f0ffff</v>
       </c>
       <c r="C239">
         <v>245.23599999999999</v>
@@ -6063,8 +6428,9 @@
       <c r="A240">
         <v>19</v>
       </c>
-      <c r="B240" t="s">
-        <v>32</v>
+      <c r="B240" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C240">
         <v>245.23599999999999</v>
@@ -20476,7 +20842,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K338"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -20514,7 +20880,7 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>